<commit_message>
change made to excel file
</commit_message>
<xml_diff>
--- a/BddFrameworkGherkin/automation.xlsx
+++ b/BddFrameworkGherkin/automation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgajdosz\Documents\bench learning\BDD\greg\CucumberTestAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgajdosz\Documents\bench learning\BDD\Gherkin-Cucumber\BddFrameworkGherkin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD4E8E4-26A7-4E42-A3D2-CAF7695706F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC863657-A00F-4658-987E-EC79E6040E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D49A02D6-1CAD-4228-9FE1-F8829C14B003}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D49A02D6-1CAD-4228-9FE1-F8829C14B003}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -33,18 +33,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>Greg</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Clint</t>
-  </si>
-  <si>
-    <t>Roman</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -52,6 +40,24 @@
   </si>
   <si>
     <t>Condition</t>
+  </si>
+  <si>
+    <t>mngr322726</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Eli</t>
+  </si>
+  <si>
+    <t>ratahYn</t>
+  </si>
+  <si>
+    <t>asfd</t>
+  </si>
+  <si>
+    <t>asdratahYn</t>
   </si>
 </sst>
 </file>
@@ -406,7 +412,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -423,51 +429,51 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3">
-        <v>12345</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>12345</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>12346</v>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>